<commit_message>
feat: Add MAL agg packages for v 2.35, 2.36; update for v 2.33, 2.34
</commit_message>
<xml_diff>
--- a/metadata/MAL/MAL-HIST_CUSTOM_V1_DHIS2.33/reference.xlsx
+++ b/metadata/MAL/MAL-HIST_CUSTOM_V1_DHIS2.33/reference.xlsx
@@ -420,13 +420,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -458,7 +458,7 @@
         <v>Version</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>V1.1.0</v>
+        <v>1.1.0</v>
       </c>
     </row>
     <row r="5">
@@ -466,23 +466,31 @@
         <v>DHIS2 version</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>DHIS2.33</v>
+        <v>2.33.9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>Created</v>
+        <v>DHIS2 build</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2020-09-12T16:58</v>
+        <v>58094d2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>Identifier</v>
+        <v>Last updated</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>MAL-HIST_CUSTOM_V1.1.0_DHIS2.33_2020-09-12T16:58</v>
+        <v>20210520T090044</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="str">
+        <v>Name</v>
+      </c>
+      <c r="B8" s="4" t="str">
+        <v>MAL-HIST_CUSTOM_V1.1.0_2.33.9-en</v>
       </c>
     </row>
   </sheetData>
@@ -764,16 +772,16 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>MAL - Malaria confirmed cases (Mic+RDT)</v>
+        <v>MAL - Plasmodium falciparum (Mic+RDT)</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>Positive (micr+RDT)</v>
+        <v>P. falciparum (micr+RDT)</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>MAL_CONFI_CASES_MICR_RDT</v>
+        <v>MAL_PF_MICR_RDT</v>
       </c>
       <c r="D2" s="4" t="str">
-        <v>Cases confirmed as positive with microscopy and/or RDT</v>
+        <v>Cases confirmed as P.falciparum positive with microscopy and/or RDT</v>
       </c>
       <c r="E2" s="4" t="str">
         <v>IvYR8mc6prX</v>
@@ -782,21 +790,21 @@
         <v>2019-10-20</v>
       </c>
       <c r="G2" s="4" t="str">
-        <v>X0luAFiy268</v>
+        <v>IIU1O0Z4l49</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
-        <v>MAL - Malaria tested cases (Mic+RDT)</v>
+        <v>MAL - Mixed/Other malaria species (Mic+RDT)</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>Tested (micr+RDT)</v>
+        <v>Other species (micr+RDT)</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>MAL_TEST_CASES_MICR_RDT</v>
+        <v>MAL_MIX_OTHER_SPECIES_MICR_RDT</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>Suspected cases tested with both microscopy and/or RDT</v>
+        <v>Cases confirmed as P.malariae or P. ovale or P. knowlesi with microscopy and/or RDT</v>
       </c>
       <c r="E3" s="5" t="str">
         <v>IvYR8mc6prX</v>
@@ -805,21 +813,21 @@
         <v>2019-10-20</v>
       </c>
       <c r="G3" s="5" t="str">
-        <v>tuOTgWfDO6m</v>
+        <v>JkOyLRb3dpX</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>MAL - Mixed malaria species  (Mic+RDT)</v>
+        <v>MAL - Plasmodium vivax (Mic+RDT)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>Mixed (micr+RDT)</v>
+        <v>P. vivax (micr+RDT)</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>MAL_MIX_SPECIES_MICR_RDT</v>
+        <v>MAL_PV_MICR_RDT</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>Cases confirmed as mixed infection with P.falciparum and P.vivax with microscopy and/or RDT</v>
+        <v>Cases confirmed as P.vivax positive with microscopy</v>
       </c>
       <c r="E4" s="4" t="str">
         <v>IvYR8mc6prX</v>
@@ -828,21 +836,21 @@
         <v>2019-10-20</v>
       </c>
       <c r="G4" s="4" t="str">
-        <v>TNTW2ruEVEu</v>
+        <v>pUC8tgzn0lV</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="str">
-        <v>MAL - Mixed/Other malaria species (Mic+RDT)</v>
+        <v>MAL - Mixed malaria species  (Mic+RDT)</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>Other species (micr+RDT)</v>
+        <v>Mixed (micr+RDT)</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>MAL_MIX_OTHER_SPECIES_MICR_RDT</v>
+        <v>MAL_MIX_SPECIES_MICR_RDT</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>Cases confirmed as P.malariae or P. ovale or P. knowlesi with microscopy and/or RDT</v>
+        <v>Cases confirmed as mixed infection with P.falciparum and P.vivax with microscopy and/or RDT</v>
       </c>
       <c r="E5" s="5" t="str">
         <v>IvYR8mc6prX</v>
@@ -851,21 +859,21 @@
         <v>2019-10-20</v>
       </c>
       <c r="G5" s="5" t="str">
-        <v>JkOyLRb3dpX</v>
+        <v>TNTW2ruEVEu</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>MAL - Plasmodium falciparum (Mic+RDT)</v>
+        <v>MAL - Malaria tested cases (Mic+RDT)</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>P. falciparum (micr+RDT)</v>
+        <v>Tested (micr+RDT)</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>MAL_PF_MICR_RDT</v>
+        <v>MAL_TEST_CASES_MICR_RDT</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>Cases confirmed as P.falciparum positive with microscopy and/or RDT</v>
+        <v>Suspected cases tested with both microscopy and/or RDT</v>
       </c>
       <c r="E6" s="4" t="str">
         <v>IvYR8mc6prX</v>
@@ -874,21 +882,21 @@
         <v>2019-10-20</v>
       </c>
       <c r="G6" s="4" t="str">
-        <v>IIU1O0Z4l49</v>
+        <v>tuOTgWfDO6m</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>MAL - Plasmodium vivax (Mic+RDT)</v>
+        <v>MAL - Malaria confirmed cases (Mic+RDT)</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>P. vivax (micr+RDT)</v>
+        <v>Positive (micr+RDT)</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>MAL_PV_MICR_RDT</v>
+        <v>MAL_CONFI_CASES_MICR_RDT</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>Cases confirmed as P.vivax positive with microscopy</v>
+        <v>Cases confirmed as positive with microscopy and/or RDT</v>
       </c>
       <c r="E7" s="5" t="str">
         <v>IvYR8mc6prX</v>
@@ -897,7 +905,7 @@
         <v>2019-10-20</v>
       </c>
       <c r="G7" s="5" t="str">
-        <v>pUC8tgzn0lV</v>
+        <v>X0luAFiy268</v>
       </c>
     </row>
   </sheetData>
@@ -928,7 +936,7 @@
         <v>Malaria old records only</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>MAL - Malaria tested cases (Mic+RDT)</v>
+        <v>MAL - Plasmodium falciparum (Mic+RDT)</v>
       </c>
     </row>
     <row r="3">
@@ -936,7 +944,7 @@
         <v>Malaria old records only</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>MAL - Mixed malaria species  (Mic+RDT)</v>
+        <v>MAL - Mixed/Other malaria species (Mic+RDT)</v>
       </c>
     </row>
     <row r="4">
@@ -952,7 +960,7 @@
         <v>Malaria old records only</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>MAL - Malaria confirmed cases (Mic+RDT)</v>
+        <v>MAL - Mixed malaria species  (Mic+RDT)</v>
       </c>
     </row>
     <row r="6">
@@ -960,7 +968,7 @@
         <v>Malaria old records only</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>MAL - Plasmodium falciparum (Mic+RDT)</v>
+        <v>MAL - Malaria tested cases (Mic+RDT)</v>
       </c>
     </row>
     <row r="7">
@@ -968,7 +976,7 @@
         <v>Malaria old records only</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>MAL - Mixed/Other malaria species (Mic+RDT)</v>
+        <v>MAL - Malaria confirmed cases (Mic+RDT)</v>
       </c>
     </row>
   </sheetData>
@@ -1000,13 +1008,13 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="str">
-        <v>Malaria access</v>
+        <v>Malaria data capture</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2020-04-24</v>
+        <v>2021-05-20</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>ZXEVDM9XRea</v>
+        <v>fRSrUJ6SMGH</v>
       </c>
     </row>
     <row r="3">
@@ -1014,7 +1022,7 @@
         <v>Malaria admin</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2020-09-03</v>
+        <v>2021-05-20</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>suMb19wGXPR</v>
@@ -1022,13 +1030,13 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="str">
-        <v>Malaria data capture</v>
+        <v>Malaria access</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2020-04-24</v>
+        <v>2021-05-20</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>fRSrUJ6SMGH</v>
+        <v>ZXEVDM9XRea</v>
       </c>
     </row>
   </sheetData>

</xml_diff>